<commit_message>
Semi-final changes, day 1
</commit_message>
<xml_diff>
--- a/data/mistakes/Morfeusz_lemma_mistakes.xlsx
+++ b/data/mistakes/Morfeusz_lemma_mistakes.xlsx
@@ -2571,7 +2571,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
@@ -7021,7 +7021,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>oyca</t>
+          <t>oyciec</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">

</xml_diff>